<commit_message>
Uses cases presque terminés
</commit_message>
<xml_diff>
--- a/Projet/Documentation/journal de travail.xlsx
+++ b/Projet/Documentation/journal de travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Mise en place de Git, réinstallation de python et PyCharm, création et clonage d'un repository dédié, mise en place de l'arborescence de travail de base</t>
   </si>
   <si>
-    <t>Heures de travail totales</t>
-  </si>
-  <si>
     <t>Téléchargement de différents fichiers</t>
   </si>
   <si>
@@ -81,6 +78,18 @@
   </si>
   <si>
     <t>Création du journal de travail</t>
+  </si>
+  <si>
+    <t>mar 15.05</t>
+  </si>
+  <si>
+    <t>Création des Use-case &amp; Scénarios</t>
+  </si>
+  <si>
+    <t>Heures de travail totales (Selon l'horaire du CPNV)</t>
+  </si>
+  <si>
+    <t>Checerches sur tkinter</t>
   </si>
 </sst>
 </file>
@@ -88,8 +97,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
-    <numFmt numFmtId="166" formatCode="ddd/mm/yy"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="ddd/mm/yy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -208,7 +217,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -217,37 +226,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -533,7 +542,7 @@
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:C23"/>
+      <selection activeCell="A13" sqref="A13:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,7 +555,7 @@
     <col min="6" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -560,11 +569,11 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
+      <c r="A2" s="11">
         <v>43228.05</v>
       </c>
       <c r="B2" s="4">
@@ -574,225 +583,253 @@
         <v>4</v>
       </c>
       <c r="D2" s="5"/>
-      <c r="E2" s="6">
+      <c r="E2" s="14">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="7">
+      <c r="A3" s="12"/>
+      <c r="B3" s="6">
         <v>0.5</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="9"/>
+      <c r="E3" s="15"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="7">
+      <c r="A4" s="12"/>
+      <c r="B4" s="6">
         <v>0.5</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="E4" s="15"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="9"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="C5" s="8" t="s">
+      <c r="D5" s="7"/>
+      <c r="E5" s="15"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
+      <c r="B6" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="9"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="10">
-        <v>1.5</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="16"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
+      <c r="A7" s="11">
         <v>43229</v>
       </c>
       <c r="B7" s="4">
         <v>1.5</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+      <c r="B8" s="6">
+        <v>2</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="7">
+      <c r="D8" s="7"/>
+      <c r="E8" s="15"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="15"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="6">
         <v>2</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="9"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="7">
-        <v>0.75</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="9"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="7">
+      <c r="D10" s="7"/>
+      <c r="E10" s="15"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="6">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="15"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="16"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="4">
         <v>2</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="7">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="9"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="12"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="15"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="16"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
+      <c r="A16" s="10"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
+      <c r="A17" s="10"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
+      <c r="A18" s="10"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
+      <c r="A19" s="10"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
+      <c r="A20" s="10"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
+      <c r="A21" s="10"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
+      <c r="A22" s="10"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
+      <c r="A23" s="10"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
+      <c r="A24" s="10"/>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
+      <c r="A25" s="10"/>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
+      <c r="A26" s="10"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
+      <c r="A27" s="10"/>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
+      <c r="A28" s="10"/>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
+      <c r="A29" s="10"/>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
+      <c r="A30" s="10"/>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
+      <c r="A31" s="10"/>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="16"/>
+      <c r="A32" s="10"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="16"/>
+      <c r="A33" s="10"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="16"/>
+      <c r="A34" s="10"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
+      <c r="A35" s="10"/>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="16"/>
+      <c r="A36" s="10"/>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="16"/>
+      <c r="A37" s="10"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="16"/>
+      <c r="A38" s="10"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="16"/>
+      <c r="A39" s="10"/>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="16"/>
+      <c r="A40" s="10"/>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="16"/>
+      <c r="A41" s="10"/>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="16"/>
+      <c r="A42" s="10"/>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="16"/>
+      <c r="A43" s="10"/>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="16"/>
+      <c r="A44" s="10"/>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
@@ -804,11 +841,13 @@
       <c r="A47" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="E2:E6"/>
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="E7:E12"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="E13:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Début de l'interface graphique, doc mise à jour
Début du développement de l'interface graphique grâce à tkinter
</commit_message>
<xml_diff>
--- a/Projet/Documentation/journal de travail.xlsx
+++ b/Projet/Documentation/journal de travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -90,6 +90,15 @@
   </si>
   <si>
     <t>Checerches sur tkinter</t>
+  </si>
+  <si>
+    <t>Finalisation des use-case &amp; scénarios</t>
+  </si>
+  <si>
+    <t>Création de l'application de base</t>
+  </si>
+  <si>
+    <t>Mise en place d'un fichier de config, création d'une classe "Main_Window", et création d'un semblant d'interface grâce à tkinter</t>
   </si>
 </sst>
 </file>
@@ -542,7 +551,7 @@
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:E15"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,54 +754,74 @@
       <c r="E15" s="16"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>43236</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
+        <v>3</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="10"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Images d'entraînement ajoutées, début d'interface
Concept d'interface, non fonctionnel, cela dit mon travail avance dans la bonne direction.
</commit_message>
<xml_diff>
--- a/Projet/Documentation/journal de travail.xlsx
+++ b/Projet/Documentation/journal de travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -99,15 +99,35 @@
   </si>
   <si>
     <t>Mise en place d'un fichier de config, création d'une classe "Main_Window", et création d'un semblant d'interface grâce à tkinter</t>
+  </si>
+  <si>
+    <t>Tentatives d'installation du package de gestion d'images Pillow</t>
+  </si>
+  <si>
+    <t>Début de la création de l'interface tkinter</t>
+  </si>
+  <si>
+    <t>Problèmes d'importation de la librairie pillow, permettant notamment la gestion d'images jpg et png en python</t>
+  </si>
+  <si>
+    <t>Résolution du problème relatif à Pillow</t>
+  </si>
+  <si>
+    <t>L'installation de la distribution "Anaconda" a réglé mon probleme</t>
+  </si>
+  <si>
+    <t>Développement de l'interface</t>
+  </si>
+  <si>
+    <t>Gestion d'image, boutons, le placement des éléments avec tkinter est retors, mais ne devrait pas poser de problèmes longtemps. J'ai pu améliorer mes compétences sur tkinter grâce à pygubu, un générateur d'interface, que j'ai utilisé pour comprendre le fonctionnement de la grille de tkinter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
-    <numFmt numFmtId="165" formatCode="ddd/mm/yy"/>
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="ddd\ dd/mm/yy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -218,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -226,9 +246,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -247,18 +264,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -267,6 +272,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -550,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,295 +599,351 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
+      <c r="A2" s="12">
         <v>43228.05</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>1.5</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="14">
+      <c r="D2" s="4"/>
+      <c r="E2" s="9">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="6">
+      <c r="A3" s="13"/>
+      <c r="B3" s="5">
         <v>0.5</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="15"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="6">
+      <c r="A4" s="13"/>
+      <c r="B4" s="5">
         <v>0.5</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="15"/>
+      <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="6">
+      <c r="A5" s="13"/>
+      <c r="B5" s="5">
         <v>0.5</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="15"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="8">
+      <c r="A6" s="14"/>
+      <c r="B6" s="7">
         <v>1.5</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="16"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
+      <c r="A7" s="12">
         <v>43229</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>1.5</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="14">
+      <c r="D7" s="4"/>
+      <c r="E7" s="9">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="6">
+      <c r="A8" s="13"/>
+      <c r="B8" s="5">
         <v>2</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="15"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="10"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="6">
+      <c r="A9" s="13"/>
+      <c r="B9" s="5">
         <v>0.75</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="15"/>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="6">
+      <c r="A10" s="13"/>
+      <c r="B10" s="5">
         <v>2</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="15"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="10"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="6">
+      <c r="A11" s="13"/>
+      <c r="B11" s="5">
         <v>1.1499999999999999</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="15"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="10"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="8">
+      <c r="A12" s="14"/>
+      <c r="B12" s="7">
         <v>0.5</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="16"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="11"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>2</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="14">
+      <c r="D13" s="4"/>
+      <c r="E13" s="9">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="6">
+      <c r="A14" s="13"/>
+      <c r="B14" s="5">
         <v>1.5</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="15"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="10"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
-      <c r="B15" s="8">
+      <c r="B15" s="7">
         <v>1.5</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="16"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="11"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
+      <c r="A16" s="12">
         <v>43236</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="3">
         <v>0.5</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="2">
+      <c r="D16" s="4"/>
+      <c r="E16" s="9">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="1">
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="5">
         <v>3</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
+      <c r="E17" s="10"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="7">
+        <v>3</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="11"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
+        <v>43237</v>
+      </c>
+      <c r="B20" s="3">
+        <v>2</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="7">
+        <v>7</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="11"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="15"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="15"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="12">
+        <v>43238</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="13"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="13"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="12"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="13"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="13"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="13"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="12"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
+      <c r="A33" s="13"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
+      <c r="A34" s="13"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="10"/>
+      <c r="A35" s="13"/>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="10"/>
+      <c r="A36" s="12"/>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="10"/>
+      <c r="A37" s="13"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="10"/>
+      <c r="A38" s="13"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="10"/>
+      <c r="A39" s="13"/>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="10"/>
+      <c r="A40" s="12"/>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="10"/>
+      <c r="A41" s="13"/>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="10"/>
+      <c r="A42" s="13"/>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="10"/>
+      <c r="A43" s="13"/>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="10"/>
+      <c r="A44" s="12"/>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
+      <c r="A45" s="13"/>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
+      <c r="A46" s="13"/>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
+      <c r="A47" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="16">
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="E20:E21"/>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="E2:E6"/>
     <mergeCell ref="A7:A12"/>

</xml_diff>

<commit_message>
Avancement de l'interface, travail sur l'outil de sélection
</commit_message>
<xml_diff>
--- a/Projet/Documentation/journal de travail.xlsx
+++ b/Projet/Documentation/journal de travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Création du journal de travail</t>
   </si>
   <si>
-    <t>mar 15.05</t>
-  </si>
-  <si>
     <t>Création des Use-case &amp; Scénarios</t>
   </si>
   <si>
@@ -120,6 +117,18 @@
   </si>
   <si>
     <t>Gestion d'image, boutons, le placement des éléments avec tkinter est retors, mais ne devrait pas poser de problèmes longtemps. J'ai pu améliorer mes compétences sur tkinter grâce à pygubu, un générateur d'interface, que j'ai utilisé pour comprendre le fonctionnement de la grille de tkinter</t>
+  </si>
+  <si>
+    <t>mar 15.05.18</t>
+  </si>
+  <si>
+    <t>Suite du développement de l'interface</t>
+  </si>
+  <si>
+    <t>Presque tous les boutons sont fonctionnels, j'ai récupéré quelques paragraphes de code qui me permettent de dessiner une boîte de sélection dans le canvas, et grâce à la librairie PIL, j'arrive à prendre un screenshot aux coordonnées se trouvant dans la selection box</t>
+  </si>
+  <si>
+    <t>Développement de la boîte de sélection</t>
   </si>
 </sst>
 </file>
@@ -127,7 +136,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="ddd\ dd/mm/yy"/>
+    <numFmt numFmtId="164" formatCode="ddd\ dd/mm/yy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -238,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -264,6 +273,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -273,16 +291,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -567,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:A27"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,11 +607,11 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
+      <c r="A2" s="10">
         <v>43228.05</v>
       </c>
       <c r="B2" s="3">
@@ -609,12 +621,12 @@
         <v>4</v>
       </c>
       <c r="D2" s="4"/>
-      <c r="E2" s="9">
+      <c r="E2" s="12">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
+      <c r="A3" s="11"/>
       <c r="B3" s="5">
         <v>0.5</v>
       </c>
@@ -624,10 +636,10 @@
       <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="10"/>
+      <c r="E3" s="13"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="5">
         <v>0.5</v>
       </c>
@@ -637,10 +649,10 @@
       <c r="D4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="10"/>
+      <c r="E4" s="13"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="5">
         <v>0.5</v>
       </c>
@@ -648,10 +660,10 @@
         <v>9</v>
       </c>
       <c r="D5" s="6"/>
-      <c r="E5" s="10"/>
+      <c r="E5" s="13"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="7">
         <v>1.5</v>
       </c>
@@ -659,10 +671,10 @@
         <v>10</v>
       </c>
       <c r="D6" s="8"/>
-      <c r="E6" s="11"/>
+      <c r="E6" s="14"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
+      <c r="A7" s="10">
         <v>43229</v>
       </c>
       <c r="B7" s="3">
@@ -672,12 +684,12 @@
         <v>11</v>
       </c>
       <c r="D7" s="4"/>
-      <c r="E7" s="9">
+      <c r="E7" s="12">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
+      <c r="A8" s="11"/>
       <c r="B8" s="5">
         <v>2</v>
       </c>
@@ -685,10 +697,10 @@
         <v>12</v>
       </c>
       <c r="D8" s="6"/>
-      <c r="E8" s="10"/>
+      <c r="E8" s="13"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="5">
         <v>0.75</v>
       </c>
@@ -698,10 +710,10 @@
       <c r="D9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="10"/>
+      <c r="E9" s="13"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
+      <c r="A10" s="11"/>
       <c r="B10" s="5">
         <v>2</v>
       </c>
@@ -709,10 +721,10 @@
         <v>15</v>
       </c>
       <c r="D10" s="6"/>
-      <c r="E10" s="10"/>
+      <c r="E10" s="13"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
+      <c r="A11" s="11"/>
       <c r="B11" s="5">
         <v>1.1499999999999999</v>
       </c>
@@ -720,10 +732,10 @@
         <v>16</v>
       </c>
       <c r="D11" s="6"/>
-      <c r="E11" s="10"/>
+      <c r="E11" s="13"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="7">
         <v>0.5</v>
       </c>
@@ -731,25 +743,25 @@
         <v>17</v>
       </c>
       <c r="D12" s="8"/>
-      <c r="E12" s="11"/>
+      <c r="E12" s="14"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
-        <v>18</v>
+      <c r="A13" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="B13" s="3">
         <v>2</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" s="4"/>
-      <c r="E13" s="9">
+      <c r="E13" s="12">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="5">
         <v>1.5</v>
       </c>
@@ -757,199 +769,215 @@
         <v>16</v>
       </c>
       <c r="D14" s="6"/>
-      <c r="E14" s="10"/>
+      <c r="E14" s="13"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="7">
         <v>1.5</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D15" s="8"/>
-      <c r="E15" s="11"/>
+      <c r="E15" s="14"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
+      <c r="A16" s="10">
         <v>43236</v>
       </c>
       <c r="B16" s="3">
         <v>0.5</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16" s="4"/>
-      <c r="E16" s="9">
+      <c r="E16" s="12">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="5">
         <v>3</v>
       </c>
       <c r="C17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E17" s="10"/>
+      <c r="E17" s="13"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="5">
         <v>2.5</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D18" s="6"/>
-      <c r="E18" s="10"/>
+      <c r="E18" s="13"/>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
+      <c r="A19" s="11"/>
       <c r="B19" s="7">
         <v>3</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="11"/>
+        <v>26</v>
+      </c>
+      <c r="E19" s="14"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="12">
+      <c r="A20" s="10">
         <v>43237</v>
       </c>
       <c r="B20" s="3">
         <v>2</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E20" s="9">
+      <c r="E20" s="12">
         <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
+      <c r="A21" s="15"/>
       <c r="B21" s="7">
         <v>7</v>
       </c>
       <c r="C21" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21" s="11"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
+      <c r="E21" s="14"/>
+    </row>
+    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
+        <v>43238</v>
+      </c>
+      <c r="B22" s="3">
+        <v>3</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="12">
+        <v>7</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
+      <c r="B23" s="7">
+        <v>4</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="14"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="12">
-        <v>43238</v>
-      </c>
+      <c r="A24" s="9"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
+      <c r="A25" s="9"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
+      <c r="A26" s="9"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
+      <c r="A27" s="9"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
+      <c r="A28" s="9"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
+      <c r="A29" s="16"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
+      <c r="A30" s="16"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
+      <c r="A31" s="16"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
+      <c r="A32" s="16"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
+      <c r="A33" s="16"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
+      <c r="A34" s="16"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
+      <c r="A35" s="16"/>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
+      <c r="A36" s="16"/>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="13"/>
+      <c r="A37" s="16"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="13"/>
+      <c r="A38" s="16"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
+      <c r="A39" s="16"/>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
+      <c r="A40" s="16"/>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="13"/>
+      <c r="A41" s="16"/>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="13"/>
+      <c r="A42" s="16"/>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="13"/>
+      <c r="A43" s="16"/>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="12"/>
+      <c r="A44" s="16"/>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="13"/>
+      <c r="A45" s="9"/>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="13"/>
+      <c r="A46" s="9"/>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="13"/>
+      <c r="A47" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="E16:E19"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="E20:E21"/>
+  <mergeCells count="12">
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="E2:E6"/>
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="E7:E12"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="E13:E15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="E22:E23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>